<commit_message>
Add Class: Passive Load
</commit_message>
<xml_diff>
--- a/CustomerData/netlist.xlsx
+++ b/CustomerData/netlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\CustomerData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5F22CF-B9D6-45A5-BDDD-A71E41D08512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B72185-3D79-4680-826E-432C8E278ACE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PowerFlow" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t>bus</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -214,10 +214,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>The buses CAN be listed below in arbitrary order.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Discretization Method</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -258,51 +254,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>10-19, Grid-Following VSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20-29, Grid-Forming VSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21, Droop-Controlled VSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zbranch = R+wL+1/(wC+G)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0-10, Synchronous Generator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>R (pu)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>L (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>90, RL Load</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>90-99, Load</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>91, PQ Load</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10-19, Grid-Following VSI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20-29, Grid-Forming VSI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>21, Droop-Controlled VSI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zbranch = R+wL+1/(wC+G)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0-10, Synchronous Generator</t>
+    <t>Notes:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>91, RL Load</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PQ value is obtained from "PowerFlow"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For load, only types 90, 91 are available for use now. Other types will be added later.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>90-99, Passive Load</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>90, PQ Passive Load</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>92, RLC Load</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Connection (1-Series, 2-Parallel)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P and Q are in generator convention.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For PQ Load bus, P and Q have to be negative.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -661,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -686,89 +698,62 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>3</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>5</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" t="s">
         <v>6</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" t="s">
         <v>7</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I8" t="s">
         <v>8</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J8" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0.5</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>-1</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -797,7 +782,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -829,10 +814,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -844,7 +829,7 @@
         <v>0.5</v>
       </c>
       <c r="F11">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -856,6 +841,38 @@
         <v>-1</v>
       </c>
       <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0.5</v>
+      </c>
+      <c r="F12">
+        <v>-0.2</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>-1</v>
+      </c>
+      <c r="J12">
         <v>1</v>
       </c>
     </row>
@@ -870,7 +887,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -887,7 +904,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
@@ -1104,16 +1121,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10.86328125" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="2" max="2" width="31.59765625" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" customWidth="1"/>
+    <col min="4" max="4" width="12.1328125" customWidth="1"/>
+    <col min="5" max="5" width="11.19921875" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.86328125" customWidth="1"/>
+    <col min="8" max="8" width="19.19921875" customWidth="1"/>
+    <col min="9" max="9" width="19.06640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
@@ -1143,8 +1167,8 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
-      <c r="B6" t="s">
-        <v>66</v>
+      <c r="B6" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
@@ -1167,8 +1191,8 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="3"/>
-      <c r="B8" t="s">
-        <v>62</v>
+      <c r="B8" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
@@ -1201,31 +1225,31 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
-      <c r="B12" t="s">
-        <v>60</v>
+      <c r="B12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
       <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
@@ -1233,76 +1257,92 @@
       <c r="B14" t="s">
         <v>61</v>
       </c>
-      <c r="C14" t="s">
-        <v>57</v>
-      </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="3"/>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A16" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A17" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A18">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A21">
         <v>2</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A22">
         <v>3</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2">
         <f>3.5/10</f>
         <v>0.35</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A20">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A23">
         <v>4</v>
       </c>
-      <c r="B20">
+      <c r="B23">
         <v>10</v>
       </c>
     </row>
@@ -1317,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB93A31-1E5A-4104-8C10-8E6599437516}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1332,7 +1372,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -1342,17 +1382,17 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
@@ -1362,22 +1402,22 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
         <v>47</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Add Class: Passive Load for Simulation
</commit_message>
<xml_diff>
--- a/CustomerData/netlist.xlsx
+++ b/CustomerData/netlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\CustomerData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B72185-3D79-4680-826E-432C8E278ACE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D655E25-17B2-4E36-B108-FAA5E80B6A5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PowerFlow" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>bus</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -314,7 +314,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>For PQ Load bus, P and Q have to be negative.</t>
+    <t>For PQ Load bus, use Pli and Qli.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The generator and load CAN NOT be connected to the same bus, for this case, please use "NetworkLine" to set load.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -673,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="J13" sqref="A12:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -712,80 +716,53 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>4</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>5</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>6</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" t="s">
         <v>7</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I9" t="s">
         <v>8</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J9" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0.5</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>-1</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -814,7 +791,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -846,10 +823,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -861,7 +838,7 @@
         <v>0.5</v>
       </c>
       <c r="F12">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -873,12 +850,45 @@
         <v>-1</v>
       </c>
       <c r="J12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0.5</v>
+      </c>
+      <c r="F13">
+        <v>-0.2</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>-1</v>
+      </c>
+      <c r="J13">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -887,7 +897,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F17" sqref="A14:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1123,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1357,7 +1367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB93A31-1E5A-4104-8C10-8E6599437516}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add Class: Floating Bus
</commit_message>
<xml_diff>
--- a/CustomerData/netlist.xlsx
+++ b/CustomerData/netlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\CustomerData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D655E25-17B2-4E36-B108-FAA5E80B6A5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0E4E04-963A-4335-BB78-C4787CD29A43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t>bus</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -319,6 +319,10 @@
   </si>
   <si>
     <t>The generator and load CAN NOT be connected to the same bus, for this case, please use "NetworkLine" to set load.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100, Floating Bus</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -680,7 +684,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="A12:J13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -897,7 +901,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="A14:F17"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1131,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1281,49 +1285,40 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A17" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A18" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1338,21 +1333,36 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A23">
         <v>3</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
         <f>3.5/10</f>
         <v>0.35</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A23">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A24">
         <v>4</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Function: Load Bus
</commit_message>
<xml_diff>
--- a/CustomerData/netlist.xlsx
+++ b/CustomerData/netlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\CustomerData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0E4E04-963A-4335-BB78-C4787CD29A43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471EDF78-2C53-4241-B22B-65BCAFA3100B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PowerFlow" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>bus</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -319,10 +319,6 @@
   </si>
   <si>
     <t>The generator and load CAN NOT be connected to the same bus, for this case, please use "NetworkLine" to set load.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100, Floating Bus</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -683,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -901,7 +897,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1135,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1285,40 +1281,49 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
-        <v>71</v>
+      <c r="A16" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A17" s="3" t="s">
-        <v>60</v>
+      <c r="A17" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A18" s="5" t="s">
-        <v>63</v>
+      <c r="A18" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19" s="3" t="s">
-        <v>31</v>
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
-      </c>
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1333,36 +1338,21 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="C22" s="2">
+        <f>3.5/10</f>
+        <v>0.35</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2">
-        <f>3.5/10</f>
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A24">
-        <v>4</v>
-      </c>
-      <c r="B24">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Function: Capacitive Load
</commit_message>
<xml_diff>
--- a/CustomerData/netlist.xlsx
+++ b/CustomerData/netlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\CustomerData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B578AAC-FBD3-4FF6-A65F-CF3697E50212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D70A26-909A-4EFA-9531-2BFDDC6FE85F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
   <si>
     <t>bus</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -290,10 +290,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>For load, only types 90, 91 are available for use now. Other types will be added later.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>90-99, Passive Load</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -310,23 +306,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>P and Q are in generator convention.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>For PQ Load bus, use Pli and Qli.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The generator and load CAN NOT be connected to the same bus, for this case, please use "NetworkLine" to set load.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>100, Floating Bus</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>If the parameters are left to blank, the default paramters will be used.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PGi and QGi are in generator convention. PLi and QLi are in load convention.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For active device (SG, VSI, etc), please use PGI and QGi. For load, please use PLi and QLi.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>red</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> highlighted devices are not available currently.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For adding passive load, please use PLi and QLi in the "PowerFlow" sheet.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%%%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Default</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -337,7 +369,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,6 +409,23 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -398,13 +447,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -715,62 +767,89 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>70</v>
+      <c r="A7" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
-        <v>31</v>
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J9" t="s">
-        <v>9</v>
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.5</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>-1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -799,7 +878,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -831,10 +910,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
         <v>3</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -846,7 +925,7 @@
         <v>0.5</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -858,38 +937,6 @@
         <v>-1</v>
       </c>
       <c r="J12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0.5</v>
-      </c>
-      <c r="F13">
-        <v>-0.2</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>-1</v>
-      </c>
-      <c r="J13">
         <v>1</v>
       </c>
     </row>
@@ -905,7 +952,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1139,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1180,7 +1227,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
@@ -1193,185 +1240,244 @@
       <c r="B7" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="3"/>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
+      <c r="B8" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
-      <c r="B9" s="3" t="s">
-        <v>54</v>
+      <c r="B9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" t="s">
-        <v>29</v>
+      <c r="B10" s="8" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
-      <c r="B11" t="s">
-        <v>55</v>
+      <c r="B11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>67</v>
+      <c r="B13" s="8" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
-      <c r="B14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" t="s">
-        <v>62</v>
+      <c r="B14" s="6" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
-      <c r="B15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" t="s">
-        <v>23</v>
-      </c>
+      <c r="B15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
-      <c r="B16" t="s">
-        <v>66</v>
-      </c>
+      <c r="B16" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A18" s="3"/>
+      <c r="B18" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A19" s="3"/>
+      <c r="B19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A20" s="3"/>
+      <c r="B20" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A21" s="3"/>
+      <c r="B21" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A23" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A24" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A18" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A20" s="3" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A25" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A26" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
         <v>17</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B27" t="s">
         <v>18</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A23">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A29">
         <v>2</v>
       </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A24">
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A30">
         <v>3</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24" s="2">
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2">
         <f>3.5/10</f>
         <v>0.35</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A31">
         <v>4</v>
       </c>
-      <c r="B25">
+      <c r="B31">
         <v>10</v>
       </c>
     </row>
@@ -1387,7 +1493,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>

</xml_diff>